<commit_message>
Updated IT step table
</commit_message>
<xml_diff>
--- a/Integrationplan.xlsx
+++ b/Integrationplan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\Github\Microwave\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\morte\Desktop\Microwave\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FBA2B4A-DE45-4390-86D8-7730406267E3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADA514B-5A64-497E-927C-EC7719273AF3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8EA7D682-06A8-4BAA-9350-50B723065ED3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8EA7D682-06A8-4BAA-9350-50B723065ED3}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="23">
   <si>
     <t>Step#</t>
   </si>
@@ -87,6 +87,18 @@
   </si>
   <si>
     <t>Modulet er faked</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>Start/Cancel Button</t>
+  </si>
+  <si>
+    <t>Timer Button</t>
+  </si>
+  <si>
+    <t>Power Button</t>
   </si>
 </sst>
 </file>
@@ -518,7 +530,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -814,20 +826,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF12CA7-1099-4869-950E-143932C57D3F}">
-  <dimension ref="B1:O25"/>
+  <dimension ref="B1:XFD1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23:O25"/>
+    <sheetView tabSelected="1" zoomScale="123" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
     <col min="15" max="15" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -859,7 +872,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6">
         <v>1</v>
       </c>
@@ -889,7 +902,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="19">
         <v>2</v>
       </c>
@@ -915,7 +928,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="10">
         <v>3</v>
       </c>
@@ -939,7 +952,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="19">
         <v>4</v>
       </c>
@@ -965,7 +978,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10">
         <v>5</v>
       </c>
@@ -985,7 +998,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="19">
         <v>6</v>
       </c>
@@ -1005,7 +1018,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:11" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14">
         <v>7</v>
       </c>
@@ -1037,8 +1050,167 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="14:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="14:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="6">
+        <v>1</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="9"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="19">
+        <v>2</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="22"/>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="10">
+        <v>3</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="13"/>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18" s="19">
+        <v>4</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="L18" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="M18" s="22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="2:15" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="N23" s="23" t="s">
         <v>13</v>
       </c>
@@ -1046,7 +1218,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="14:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="N24" s="27" t="s">
         <v>14</v>
       </c>
@@ -1054,13 +1226,55 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="14:15" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:15" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N25" s="25" t="s">
         <v>15</v>
       </c>
       <c r="O25" s="26" t="s">
         <v>18</v>
       </c>
+    </row>
+    <row r="1048574" spans="16373:16384" x14ac:dyDescent="0.25">
+      <c r="XES1048574" s="10"/>
+      <c r="XET1048574" s="12"/>
+      <c r="XEU1048574" s="11"/>
+      <c r="XEV1048574" s="12"/>
+      <c r="XEW1048574" s="12"/>
+      <c r="XEX1048574" s="12"/>
+      <c r="XEY1048574" s="12"/>
+      <c r="XEZ1048574" s="12"/>
+      <c r="XFA1048574" s="12"/>
+      <c r="XFB1048574" s="12"/>
+      <c r="XFC1048574" s="12"/>
+      <c r="XFD1048574" s="13"/>
+    </row>
+    <row r="1048575" spans="16373:16384" x14ac:dyDescent="0.25">
+      <c r="XES1048575" s="19"/>
+      <c r="XET1048575" s="21"/>
+      <c r="XEU1048575" s="20"/>
+      <c r="XEV1048575" s="21"/>
+      <c r="XEW1048575" s="21"/>
+      <c r="XEX1048575" s="21"/>
+      <c r="XEY1048575" s="21"/>
+      <c r="XEZ1048575" s="21"/>
+      <c r="XFA1048575" s="21"/>
+      <c r="XFB1048575" s="21"/>
+      <c r="XFC1048575" s="21"/>
+      <c r="XFD1048575" s="22"/>
+    </row>
+    <row r="1048576" spans="16373:16384" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="XES1048576" s="14"/>
+      <c r="XET1048576" s="16"/>
+      <c r="XEU1048576" s="15"/>
+      <c r="XEV1048576" s="16"/>
+      <c r="XEW1048576" s="16"/>
+      <c r="XEX1048576" s="16"/>
+      <c r="XEY1048576" s="16"/>
+      <c r="XEZ1048576" s="16"/>
+      <c r="XFA1048576" s="16"/>
+      <c r="XFB1048576" s="16"/>
+      <c r="XFC1048576" s="16"/>
+      <c r="XFD1048576" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>